<commit_message>
added smoke suite class and some respective changes
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Smoke_StudentFeature.xlsx
+++ b/src/test/resources/data/Smoke_StudentFeature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="AddStudent" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Login</t>
   </si>
@@ -45,19 +45,32 @@
   </si>
   <si>
     <t>Patronymic</t>
+  </si>
+  <si>
+    <t>GroupNumber</t>
+  </si>
+  <si>
+    <t>СhangedGroupNumber</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -92,10 +105,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -376,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,9 +405,10 @@
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -407,20 +424,25 @@
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -429,10 +451,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,9 +463,10 @@
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -456,21 +479,27 @@
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -478,7 +507,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>